<commit_message>
Added scoreboard auto ordering functionality
</commit_message>
<xml_diff>
--- a/points_tracking.xlsx
+++ b/points_tracking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,90 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-11-08 04:24:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ace</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-11-08 04:24:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nice</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-11-08 04:24:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>nice</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-11-08 04:25:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>